<commit_message>
successfully insert employee data in Employee Table
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1846,11 +1846,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="5">
-    <numFmt numFmtId="174" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="175" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="191" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="168" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -2398,15 +2398,15 @@
     <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="175" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="22" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="174" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="23" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2475,7 +2475,7 @@
     <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="191" fontId="3" fillId="0" borderId="0" xfId="19" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="19" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="48" applyFont="1" applyAlignment="1">
@@ -2939,10 +2939,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L28"/>
+  <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5"/>
@@ -2958,10 +2958,9 @@
     <col min="9" max="9" width="22.625" customWidth="1"/>
     <col min="10" max="10" width="14.125" customWidth="1"/>
     <col min="11" max="11" width="13.625" customWidth="1"/>
-    <col min="12" max="12" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:11">
       <c r="A1" s="8" t="s">
         <v>216</v>
       </c>
@@ -2995,9 +2994,8 @@
       <c r="K1" s="8" t="s">
         <v>218</v>
       </c>
-      <c r="L1" s="1"/>
-    </row>
-    <row r="2" spans="1:12">
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" s="9">
         <v>1</v>
       </c>
@@ -3032,7 +3030,7 @@
         <v>35416</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:11">
       <c r="A3" s="9">
         <v>2</v>
       </c>
@@ -3067,7 +3065,7 @@
         <v>41518</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:11">
       <c r="A4" s="9">
         <v>3</v>
       </c>
@@ -3102,7 +3100,7 @@
         <v>36647</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:11">
       <c r="A5" s="9">
         <v>4</v>
       </c>
@@ -3137,7 +3135,7 @@
         <v>38671</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:11">
       <c r="A6" s="9">
         <v>5</v>
       </c>
@@ -3172,7 +3170,7 @@
         <v>33025</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:11">
       <c r="A7" s="9">
         <v>6</v>
       </c>
@@ -3207,7 +3205,7 @@
         <v>41686</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:11">
       <c r="A8" s="9">
         <v>7</v>
       </c>
@@ -3242,7 +3240,7 @@
         <v>39417</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:11">
       <c r="A9" s="9">
         <v>8</v>
       </c>
@@ -3277,7 +3275,7 @@
         <v>37849</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:11">
       <c r="A10" s="9">
         <v>9</v>
       </c>
@@ -3312,7 +3310,7 @@
         <v>39918</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:11">
       <c r="A11" s="9">
         <v>10</v>
       </c>
@@ -3347,7 +3345,7 @@
         <v>41579</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:11">
       <c r="A12" s="9">
         <v>11</v>
       </c>
@@ -3382,7 +3380,7 @@
         <v>38781</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:11">
       <c r="A13" s="9">
         <v>12</v>
       </c>
@@ -3417,7 +3415,7 @@
         <v>40858</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:11">
       <c r="A14" s="9">
         <v>13</v>
       </c>
@@ -3452,7 +3450,7 @@
         <v>41544</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:11">
       <c r="A15" s="9">
         <v>14</v>
       </c>
@@ -3487,7 +3485,7 @@
         <v>41409</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:11">
       <c r="A16" s="9">
         <v>15</v>
       </c>
@@ -3972,7 +3970,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I139"/>
   <sheetViews>
-    <sheetView topLeftCell="A106" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView topLeftCell="A79" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="H135" sqref="H135"/>
     </sheetView>
   </sheetViews>

</xml_diff>